<commit_message>
updated formatting and sizing
</commit_message>
<xml_diff>
--- a/data/Hike_Database.xlsx
+++ b/data/Hike_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meagangardner/git/DSCI_532/individual/HikeRecommendations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD831ABA-3A3C-CA43-A69E-388BDDF529AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A88D001-697E-9844-AF6D-6FE555A01A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="16660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -834,7 +834,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>-123.15461718970499</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>-122.73695394737599</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>-123.23435247622599</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>-122.47801263497701</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>-123.121757001292</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>0.13699999999999998</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>120</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
         <v>3</v>
@@ -2146,7 +2146,7 @@
         <v>-123.091022547375</v>
       </c>
     </row>
-    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>-123.080801889702</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>-123.38923326086299</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>-123.200063173478</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>75</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>-123.030203745522</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>81</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>-123.01404972014601</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>85</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>-121.984344437221</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>97</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>-123.04260732005601</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>98</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>-123.186474680896</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>99</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>-123.197840873503</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -4159,8 +4159,7 @@
   <autoFilter ref="A1:M82" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="6">
       <filters>
-        <filter val="10+"/>
-        <filter val="8 – 10"/>
+        <filter val="6 – 8"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>